<commit_message>
changed layout for heat sink w/ issue #1
</commit_message>
<xml_diff>
--- a/highcurrent_lvr.xlsx
+++ b/highcurrent_lvr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrychen/Documents/embedded/highcurrent_lvr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrychen/Dev/embedded/hardware/highcurrent_lvr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83936C6-3146-5F46-B937-38E2ADAD7733}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880F25F8-CD21-FC4F-8261-949A655AB4BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{7EF2E4F4-A9C6-1F46-8575-4F65A2148C23}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>R1+R2</t>
   </si>
@@ -486,7 +486,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,14 +660,20 @@
       <c r="B20">
         <v>20</v>
       </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21">
-        <f>(B20-B22)/0.02</f>
-        <v>860</v>
+        <f>(B20-B22)/D20</f>
+        <v>1720</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -752,7 +758,7 @@
         <v>25</v>
       </c>
       <c r="B31">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -761,7 +767,7 @@
       </c>
       <c r="B32">
         <f>(B30^-1*B31)^-1</f>
-        <v>0.82599999999999985</v>
+        <v>0.41299999999999992</v>
       </c>
       <c r="C32">
         <f>0.03*B30</f>

</xml_diff>